<commit_message>
Se subio la base de datos para el municipal
</commit_message>
<xml_diff>
--- a/Output/Drive/11. Red Carretera.xlsx
+++ b/Output/Drive/11. Red Carretera.xlsx
@@ -647,7 +647,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="F2" t="n">
         <v>35</v>
@@ -667,7 +667,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="F3" t="n">
         <v>86</v>
@@ -687,7 +687,7 @@
         <v>84</v>
       </c>
       <c r="E4" t="n">
-        <v>136</v>
+        <v>52</v>
       </c>
       <c r="F4" t="n">
         <v>24</v>
@@ -707,7 +707,7 @@
         <v>23</v>
       </c>
       <c r="E5" t="n">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="F5" t="n">
         <v>3</v>
@@ -727,7 +727,7 @@
         <v>29</v>
       </c>
       <c r="E6" t="n">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -747,7 +747,7 @@
         <v>15</v>
       </c>
       <c r="E7" t="n">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="F7" t="n">
         <v>36</v>
@@ -767,7 +767,7 @@
         <v>17</v>
       </c>
       <c r="E8" t="n">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="F8" t="n">
         <v>16</v>
@@ -787,7 +787,7 @@
         <v>59</v>
       </c>
       <c r="E9" t="n">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="F9" t="n">
         <v>33</v>
@@ -807,7 +807,7 @@
         <v>14</v>
       </c>
       <c r="E10" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
         <v>18</v>
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="E11" t="n">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="F11" t="n">
         <v>16</v>
@@ -847,7 +847,7 @@
         <v>20</v>
       </c>
       <c r="E12" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>10</v>
@@ -867,7 +867,7 @@
         <v>18</v>
       </c>
       <c r="E13" t="n">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="F13" t="n">
         <v>85</v>
@@ -887,7 +887,7 @@
         <v>69</v>
       </c>
       <c r="E14" t="n">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="F14" t="n">
         <v>2</v>
@@ -907,7 +907,7 @@
         <v>93</v>
       </c>
       <c r="E15" t="n">
-        <v>220</v>
+        <v>127</v>
       </c>
       <c r="F15" t="n">
         <v>20</v>
@@ -927,7 +927,7 @@
         <v>26</v>
       </c>
       <c r="E16" t="n">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="F16" t="n">
         <v>5</v>
@@ -947,7 +947,7 @@
         <v>48</v>
       </c>
       <c r="E17" t="n">
-        <v>124</v>
+        <v>76</v>
       </c>
       <c r="F17" t="n">
         <v>33</v>
@@ -967,7 +967,7 @@
         <v>26</v>
       </c>
       <c r="E18" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
         <v>20</v>
@@ -987,7 +987,7 @@
         <v>41</v>
       </c>
       <c r="E19" t="n">
-        <v>146</v>
+        <v>105</v>
       </c>
       <c r="F19" t="n">
         <v>44</v>
@@ -1007,7 +1007,7 @@
         <v>5</v>
       </c>
       <c r="E20" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F20" t="n">
         <v>7</v>
@@ -1027,7 +1027,7 @@
         <v>28</v>
       </c>
       <c r="E21" t="n">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="F21" t="n">
         <v>11</v>
@@ -1047,7 +1047,7 @@
         <v>5</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
         <v>6</v>
@@ -1067,7 +1067,7 @@
         <v>17</v>
       </c>
       <c r="E23" t="n">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="F23" t="n">
         <v>35</v>
@@ -1087,7 +1087,7 @@
         <v>41</v>
       </c>
       <c r="E24" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -1107,7 +1107,7 @@
         <v>27</v>
       </c>
       <c r="E25" t="n">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="F25" t="n">
         <v>73</v>
@@ -1127,7 +1127,7 @@
         <v>43</v>
       </c>
       <c r="E26" t="n">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="F26" t="n">
         <v>29</v>
@@ -1147,7 +1147,7 @@
         <v>30</v>
       </c>
       <c r="E27" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F27" t="n">
         <v>23</v>
@@ -1167,7 +1167,7 @@
         <v>28</v>
       </c>
       <c r="E28" t="n">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="F28" t="n">
         <v>30</v>
@@ -1187,7 +1187,7 @@
         <v>121</v>
       </c>
       <c r="E29" t="n">
-        <v>310</v>
+        <v>189</v>
       </c>
       <c r="F29" t="n">
         <v>47</v>
@@ -1207,7 +1207,7 @@
         <v>45</v>
       </c>
       <c r="E30" t="n">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="F30" t="n">
         <v>10</v>
@@ -1227,7 +1227,7 @@
         <v>165</v>
       </c>
       <c r="E31" t="n">
-        <v>189</v>
+        <v>24</v>
       </c>
       <c r="F31" t="n">
         <v>27</v>
@@ -1247,7 +1247,7 @@
         <v>26</v>
       </c>
       <c r="E32" t="n">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="F32" t="n">
         <v>5</v>
@@ -1267,7 +1267,7 @@
         <v>14</v>
       </c>
       <c r="E33" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1287,7 +1287,7 @@
         <v>28</v>
       </c>
       <c r="E34" t="n">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="F34" t="n">
         <v>2</v>
@@ -1307,7 +1307,7 @@
         <v>4</v>
       </c>
       <c r="E35" t="n">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F35" t="n">
         <v>29</v>
@@ -1327,7 +1327,7 @@
         <v>32</v>
       </c>
       <c r="E36" t="n">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="F36" t="n">
         <v>12</v>
@@ -1347,7 +1347,7 @@
         <v>31</v>
       </c>
       <c r="E37" t="n">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="F37" t="n">
         <v>5</v>
@@ -1367,7 +1367,7 @@
         <v>84</v>
       </c>
       <c r="E38" t="n">
-        <v>252</v>
+        <v>168</v>
       </c>
       <c r="F38" t="n">
         <v>130</v>
@@ -1387,7 +1387,7 @@
         <v>34</v>
       </c>
       <c r="E39" t="n">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="F39" t="n">
         <v>6</v>
@@ -1407,7 +1407,7 @@
         <v>17</v>
       </c>
       <c r="E40" t="n">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="F40" t="n">
         <v>52</v>
@@ -1427,7 +1427,7 @@
         <v>34</v>
       </c>
       <c r="E41" t="n">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="F41" t="n">
         <v>15</v>
@@ -1447,7 +1447,7 @@
         <v>9</v>
       </c>
       <c r="E42" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F42" t="n">
         <v>11</v>
@@ -1467,7 +1467,7 @@
         <v>11</v>
       </c>
       <c r="E43" t="n">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F43" t="n">
         <v>4</v>
@@ -1487,7 +1487,7 @@
         <v>16</v>
       </c>
       <c r="E44" t="n">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="F44" t="n">
         <v>27</v>
@@ -1507,7 +1507,7 @@
         <v>51</v>
       </c>
       <c r="E45" t="n">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="F45" t="n">
         <v>29</v>
@@ -1527,7 +1527,7 @@
         <v>2</v>
       </c>
       <c r="E46" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F46" t="n">
         <v>26</v>
@@ -1547,7 +1547,7 @@
         <v>87</v>
       </c>
       <c r="E47" t="n">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="F47" t="n">
         <v>18</v>
@@ -1587,7 +1587,7 @@
         <v>30</v>
       </c>
       <c r="E49" t="n">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="F49" t="n">
         <v>46</v>
@@ -1607,7 +1607,7 @@
         <v>6</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F50" t="n">
         <v>3</v>
@@ -1627,7 +1627,7 @@
         <v>17</v>
       </c>
       <c r="E51" t="n">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="F51" t="n">
         <v>31</v>
@@ -1647,7 +1647,7 @@
         <v>22</v>
       </c>
       <c r="E52" t="n">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="F52" t="n">
         <v>16</v>
@@ -1667,7 +1667,7 @@
         <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F53" t="n">
         <v>68</v>
@@ -1687,7 +1687,7 @@
         <v>77</v>
       </c>
       <c r="E54" t="n">
-        <v>265</v>
+        <v>188</v>
       </c>
       <c r="F54" t="n">
         <v>24</v>
@@ -1707,7 +1707,7 @@
         <v>16</v>
       </c>
       <c r="E55" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F55" t="n">
         <v>3</v>
@@ -1727,7 +1727,7 @@
         <v>12</v>
       </c>
       <c r="E56" t="n">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="F56" t="n">
         <v>5</v>
@@ -1747,7 +1747,7 @@
         <v>15</v>
       </c>
       <c r="E57" t="n">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="F57" t="n">
         <v>2</v>
@@ -1767,7 +1767,7 @@
         <v>10</v>
       </c>
       <c r="E58" t="n">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F58" t="n">
         <v>27</v>
@@ -1787,7 +1787,7 @@
         <v>16</v>
       </c>
       <c r="E59" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F59" t="n">
         <v>19</v>
@@ -1807,7 +1807,7 @@
         <v>35</v>
       </c>
       <c r="E60" t="n">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="F60" t="n">
         <v>17</v>
@@ -1827,7 +1827,7 @@
         <v>53</v>
       </c>
       <c r="E61" t="n">
-        <v>158</v>
+        <v>105</v>
       </c>
       <c r="F61" t="n">
         <v>26</v>
@@ -1847,7 +1847,7 @@
         <v>44</v>
       </c>
       <c r="E62" t="n">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="F62" t="n">
         <v>18</v>
@@ -1867,7 +1867,7 @@
         <v>90</v>
       </c>
       <c r="E63" t="n">
-        <v>193</v>
+        <v>103</v>
       </c>
       <c r="F63" t="n">
         <v>50</v>
@@ -1887,7 +1887,7 @@
         <v>28</v>
       </c>
       <c r="E64" t="n">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="F64" t="n">
         <v>4</v>
@@ -1907,7 +1907,7 @@
         <v>26</v>
       </c>
       <c r="E65" t="n">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="F65" t="n">
         <v>0</v>
@@ -1927,7 +1927,7 @@
         <v>12</v>
       </c>
       <c r="E66" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F66" t="n">
         <v>0</v>
@@ -1947,7 +1947,7 @@
         <v>6</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F67" t="n">
         <v>4</v>
@@ -1967,7 +1967,7 @@
         <v>58</v>
       </c>
       <c r="E68" t="n">
-        <v>182</v>
+        <v>124</v>
       </c>
       <c r="F68" t="n">
         <v>27</v>
@@ -1987,7 +1987,7 @@
         <v>19</v>
       </c>
       <c r="E69" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F69" t="n">
         <v>9</v>
@@ -2007,7 +2007,7 @@
         <v>13</v>
       </c>
       <c r="E70" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F70" t="n">
         <v>0</v>
@@ -2047,7 +2047,7 @@
         <v>8</v>
       </c>
       <c r="E72" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F72" t="n">
         <v>19</v>
@@ -2067,7 +2067,7 @@
         <v>76</v>
       </c>
       <c r="E73" t="n">
-        <v>253</v>
+        <v>177</v>
       </c>
       <c r="F73" t="n">
         <v>41</v>
@@ -2087,7 +2087,7 @@
         <v>23</v>
       </c>
       <c r="E74" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
         <v>5</v>
@@ -2107,7 +2107,7 @@
         <v>11</v>
       </c>
       <c r="E75" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F75" t="n">
         <v>18</v>
@@ -2127,7 +2127,7 @@
         <v>71</v>
       </c>
       <c r="E76" t="n">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
         <v>2</v>
@@ -2147,7 +2147,7 @@
         <v>75</v>
       </c>
       <c r="E77" t="n">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="F77" t="n">
         <v>23</v>
@@ -2167,7 +2167,7 @@
         <v>14</v>
       </c>
       <c r="E78" t="n">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F78" t="n">
         <v>15</v>
@@ -2187,7 +2187,7 @@
         <v>24</v>
       </c>
       <c r="E79" t="n">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="F79" t="n">
         <v>0</v>
@@ -2207,7 +2207,7 @@
         <v>13</v>
       </c>
       <c r="E80" t="n">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="F80" t="n">
         <v>0</v>
@@ -2227,7 +2227,7 @@
         <v>34</v>
       </c>
       <c r="E81" t="n">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="F81" t="n">
         <v>7</v>
@@ -2247,7 +2247,7 @@
         <v>21</v>
       </c>
       <c r="E82" t="n">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="F82" t="n">
         <v>43</v>
@@ -2267,7 +2267,7 @@
         <v>26</v>
       </c>
       <c r="E83" t="n">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="F83" t="n">
         <v>13</v>
@@ -2287,7 +2287,7 @@
         <v>39</v>
       </c>
       <c r="E84" t="n">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="F84" t="n">
         <v>23</v>
@@ -2307,7 +2307,7 @@
         <v>68</v>
       </c>
       <c r="E85" t="n">
-        <v>381</v>
+        <v>313</v>
       </c>
       <c r="F85" t="n">
         <v>149</v>

</xml_diff>